<commit_message>
Adjusted firmware for PIC16F1516.
</commit_message>
<xml_diff>
--- a/Hardware/Resources/PWM calculations.xlsx
+++ b/Hardware/Resources/PWM calculations.xlsx
@@ -532,9 +532,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -543,6 +540,9 @@
     <xf numFmtId="181" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="182" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -868,11 +868,11 @@
         <v>4</v>
       </c>
       <c r="B1" s="3">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="D1" s="1">
         <f>B1*1000*1000</f>
-        <v>32000000</v>
+        <v>16000000</v>
       </c>
       <c r="F1" s="1">
         <v>1</v>
@@ -901,11 +901,11 @@
         <v>3</v>
       </c>
       <c r="B2" s="2">
-        <v>255</v>
+        <v>63</v>
       </c>
       <c r="D2" s="1">
         <f>B2</f>
-        <v>255</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
@@ -945,38 +945,38 @@
       <c r="A6" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="32" t="str">
+      <c r="B6" s="31" t="str">
         <f>D6</f>
-        <v>FF</v>
+        <v>3F</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="21" t="str">
         <f>DEC2HEX(D2)</f>
-        <v>FF</v>
+        <v>3F</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="7">
         <f>D7</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D7" s="1">
         <f>FLOOR(LOG(4*(D2+1))/LOG(2),1)</f>
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="28"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="8">
         <f>D8*1000</f>
-        <v>4.8828125</v>
+        <v>19.53125</v>
       </c>
       <c r="D8" s="1">
         <f>D4/POWER(2,D7)</f>
-        <v>4.8828125E-3</v>
+        <v>1.953125E-2</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
@@ -985,11 +985,11 @@
       </c>
       <c r="B9" s="9">
         <f>D9/1000</f>
-        <v>31.25</v>
+        <v>62.5</v>
       </c>
       <c r="D9" s="1">
         <f>D1/D3/POWER(2,D7)</f>
-        <v>31250</v>
+        <v>62500</v>
       </c>
     </row>
     <row r="10" spans="1:12" s="21" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -998,12 +998,12 @@
       </c>
       <c r="B10" s="9">
         <f>D10/1000</f>
-        <v>31.25</v>
+        <v>62.5</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="21">
         <f>1/D11</f>
-        <v>31250</v>
+        <v>62500</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
@@ -1012,11 +1012,11 @@
       </c>
       <c r="B11" s="10">
         <f>D11*1000*1000</f>
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="D11" s="1">
         <f>(D2+1)*4*(1/D1)*D3</f>
-        <v>3.1999999999999999E-5</v>
+        <v>1.5999999999999999E-5</v>
       </c>
     </row>
   </sheetData>
@@ -1068,11 +1068,11 @@
       </c>
       <c r="B1" s="25">
         <f>'PWM-backlight'!B9</f>
-        <v>31.25</v>
+        <v>62.5</v>
       </c>
       <c r="D1">
         <f>B1*1000</f>
-        <v>31250</v>
+        <v>62500</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1138,27 +1138,27 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="32" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="17">
         <f>D8*1000</f>
-        <v>181.76948196435112</v>
+        <v>90.903001592568614</v>
       </c>
       <c r="D8">
         <f>2*D2*(0.5-ABS(D5-0.5))*D13*PI()/2</f>
-        <v>0.18176948196435111</v>
+        <v>9.0903001592568616E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="28"/>
-      <c r="B9" s="31">
+      <c r="A9" s="32"/>
+      <c r="B9" s="30">
         <f>D9</f>
-        <v>7.2707792785740438E-2</v>
+        <v>3.6361200637027448E-2</v>
       </c>
       <c r="D9">
         <f>D8/D7</f>
-        <v>7.2707792785740438E-2</v>
+        <v>3.6361200637027448E-2</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
@@ -1167,11 +1167,11 @@
       </c>
       <c r="B10" s="17">
         <f>D10*1000</f>
-        <v>181.76948196435112</v>
+        <v>90.903001592568614</v>
       </c>
       <c r="D10">
         <f>2*D2*0.5*D13*PI()/2</f>
-        <v>0.18176948196435111</v>
+        <v>9.0903001592568616E-2</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
@@ -1206,11 +1206,11 @@
       </c>
       <c r="B13" s="18">
         <f>-20*LOG(D13)</f>
-        <v>32.711378237397376</v>
+        <v>38.730233152418208</v>
       </c>
       <c r="D13">
         <f>1/SQRT(1+(D1/D11)^2)</f>
-        <v>2.3143609246303678E-2</v>
+        <v>1.1574129636278184E-2</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
@@ -1296,7 +1296,7 @@
   <cols>
     <col min="1" max="1" width="20.77734375" customWidth="1"/>
     <col min="2" max="2" width="12.77734375" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="29" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="28" customWidth="1"/>
     <col min="4" max="4" width="12" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1306,11 +1306,11 @@
       </c>
       <c r="B1" s="25">
         <f>'PWM-backlight'!B9</f>
-        <v>31.25</v>
+        <v>62.5</v>
       </c>
       <c r="D1">
         <f>B1*1000</f>
-        <v>31250</v>
+        <v>62500</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1376,29 +1376,29 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="32" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="17">
         <f>D8*1000</f>
-        <v>17.020277359006247</v>
-      </c>
-      <c r="C8" s="30"/>
+        <v>8.5105133850304799</v>
+      </c>
+      <c r="C8" s="29"/>
       <c r="D8">
         <f>2*D2*(0.5-ABS(D5-0.5))*D13*PI()/2</f>
-        <v>1.7020277359006249E-2</v>
+        <v>8.5105133850304805E-3</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="28"/>
-      <c r="B9" s="31">
+      <c r="A9" s="32"/>
+      <c r="B9" s="30">
         <f>D9</f>
-        <v>3.4040554718012497E-2</v>
-      </c>
-      <c r="C9" s="30"/>
+        <v>1.7021026770060961E-2</v>
+      </c>
+      <c r="C9" s="29"/>
       <c r="D9">
         <f>D8/D7</f>
-        <v>3.4040554718012497E-2</v>
+        <v>1.7021026770060961E-2</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
@@ -1407,11 +1407,11 @@
       </c>
       <c r="B10" s="17">
         <f>D10*1000</f>
-        <v>85.101386795031246</v>
+        <v>42.552566925152405</v>
       </c>
       <c r="D10">
         <f>2*D2*0.5*D13*PI()/2</f>
-        <v>8.510138679503125E-2</v>
+        <v>4.2552566925152406E-2</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
@@ -1446,11 +1446,11 @@
       </c>
       <c r="B13" s="18">
         <f>-20*LOG(D13)</f>
-        <v>39.303064880973089</v>
+        <v>45.323282358744883</v>
       </c>
       <c r="D13">
         <f>1/SQRT(1+(D1/D11)^2)</f>
-        <v>1.0835445097923658E-2</v>
+        <v>5.4179610939093592E-3</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Increased frequency and decreased filter capacitor.
</commit_message>
<xml_diff>
--- a/Hardware/Resources/PWM calculations.xlsx
+++ b/Hardware/Resources/PWM calculations.xlsx
@@ -388,7 +388,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="19">
+  <numFmts count="21">
     <numFmt numFmtId="164" formatCode="0\ &quot;bits&quot;"/>
     <numFmt numFmtId="165" formatCode="0\ &quot;MHz&quot;"/>
     <numFmt numFmtId="166" formatCode="0&quot;:1&quot;"/>
@@ -408,6 +408,8 @@
     <numFmt numFmtId="180" formatCode="0\ &quot;kΩ&quot;"/>
     <numFmt numFmtId="181" formatCode="0.0%"/>
     <numFmt numFmtId="182" formatCode="&quot;0x&quot;@"/>
+    <numFmt numFmtId="183" formatCode="0\ &quot;levels&quot;"/>
+    <numFmt numFmtId="184" formatCode="0.0\ &quot;uF&quot;"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -466,7 +468,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -543,6 +545,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="183" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -845,7 +856,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -901,11 +912,11 @@
         <v>3</v>
       </c>
       <c r="B2" s="2">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="D2" s="1">
         <f>B2</f>
-        <v>63</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
@@ -947,83 +958,95 @@
       </c>
       <c r="B6" s="31" t="str">
         <f>D6</f>
-        <v>3F</v>
+        <v>F</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="21" t="str">
         <f>DEC2HEX(D2)</f>
-        <v>3F</v>
+        <v>F</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="34" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="7">
         <f>D7</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D7" s="1">
         <f>FLOOR(LOG(4*(D2+1))/LOG(2),1)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="32"/>
-      <c r="B8" s="8">
-        <f>D8*1000</f>
-        <v>19.53125</v>
-      </c>
-      <c r="D8" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="32" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="34"/>
+      <c r="B8" s="33">
+        <f>D8</f>
+        <v>64</v>
+      </c>
+      <c r="C8" s="11"/>
+      <c r="D8" s="32">
+        <f>POWER(2,D7)</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="34"/>
+      <c r="B9" s="8">
+        <f>D9*1000</f>
+        <v>78.125</v>
+      </c>
+      <c r="D9" s="1">
         <f>D4/POWER(2,D7)</f>
-        <v>1.953125E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+        <v>7.8125E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="B9" s="9">
-        <f>D9/1000</f>
-        <v>62.5</v>
-      </c>
-      <c r="D9" s="1">
-        <f>D1/D3/POWER(2,D7)</f>
-        <v>62500</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" s="21" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="21" t="s">
-        <v>1</v>
       </c>
       <c r="B10" s="9">
         <f>D10/1000</f>
-        <v>62.5</v>
-      </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="21">
-        <f>1/D11</f>
-        <v>62500</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D10" s="1">
+        <f>D1/D3/POWER(2,D7)</f>
+        <v>250000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="21" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="10">
-        <f>D11*1000*1000</f>
-        <v>16</v>
-      </c>
-      <c r="D11" s="1">
+      <c r="B11" s="9">
+        <f>D11/1000</f>
+        <v>250</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="21">
+        <f>1/D12</f>
+        <v>250000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="10">
+        <f>D12*1000*1000</f>
+        <v>4</v>
+      </c>
+      <c r="D12" s="1">
         <f>(D2+1)*4*(1/D1)*D3</f>
-        <v>1.5999999999999999E-5</v>
+        <v>3.9999999999999998E-6</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <autoFilter ref="A1:B4"/>
   <mergeCells count="1">
-    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A7:A9"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
@@ -1051,7 +1074,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1067,12 +1090,12 @@
         <v>8</v>
       </c>
       <c r="B1" s="25">
-        <f>'PWM-backlight'!B9</f>
-        <v>62.5</v>
+        <f>'PWM-backlight'!B10</f>
+        <v>250</v>
       </c>
       <c r="D1">
         <f>B1*1000</f>
-        <v>62500</v>
+        <v>250000</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1105,11 +1128,11 @@
         <v>7</v>
       </c>
       <c r="B4" s="22">
-        <v>100</v>
+        <v>47</v>
       </c>
       <c r="D4">
         <f>B4/1000/1000</f>
-        <v>1E-4</v>
+        <v>4.6999999999999997E-5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1138,27 +1161,27 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="34" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="17">
         <f>D8*1000</f>
-        <v>90.903001592568614</v>
+        <v>48.354982932766326</v>
       </c>
       <c r="D8">
         <f>2*D2*(0.5-ABS(D5-0.5))*D13*PI()/2</f>
-        <v>9.0903001592568616E-2</v>
+        <v>4.8354982932766327E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="32"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="30">
         <f>D9</f>
-        <v>3.6361200637027448E-2</v>
+        <v>1.9341993173106531E-2</v>
       </c>
       <c r="D9">
         <f>D8/D7</f>
-        <v>3.6361200637027448E-2</v>
+        <v>1.9341993173106531E-2</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
@@ -1167,11 +1190,11 @@
       </c>
       <c r="B10" s="17">
         <f>D10*1000</f>
-        <v>90.903001592568614</v>
+        <v>48.354982932766326</v>
       </c>
       <c r="D10">
         <f>2*D2*0.5*D13*PI()/2</f>
-        <v>9.0903001592568616E-2</v>
+        <v>4.8354982932766327E-2</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
@@ -1180,11 +1203,11 @@
       </c>
       <c r="B11" s="12">
         <f>D11</f>
-        <v>723.43155950861501</v>
+        <v>1539.2160840608833</v>
       </c>
       <c r="D11">
         <f>1/(2*PI()*D3*D4)</f>
-        <v>723.43155950861501</v>
+        <v>1539.2160840608833</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1193,11 +1216,11 @@
       </c>
       <c r="B12" s="14">
         <f>D12*1000*1000</f>
-        <v>220.00000000000003</v>
+        <v>103.4</v>
       </c>
       <c r="D12">
         <f>D4*D3</f>
-        <v>2.2000000000000003E-4</v>
+        <v>1.0340000000000001E-4</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1206,11 +1229,11 @@
       </c>
       <c r="B13" s="18">
         <f>-20*LOG(D13)</f>
-        <v>38.730233152418208</v>
+        <v>44.212972940557016</v>
       </c>
       <c r="D13">
         <f>1/SQRT(1+(D1/D11)^2)</f>
-        <v>1.1574129636278184E-2</v>
+        <v>6.1567476454991964E-3</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
@@ -1219,11 +1242,11 @@
       </c>
       <c r="B14" s="19">
         <f>D14*1000</f>
-        <v>0.48338940701396838</v>
+        <v>0.22719302129656513</v>
       </c>
       <c r="D14">
         <f>(LN(1/(1-0.9))-LN(1/(1-0.1)))*D12</f>
-        <v>4.833894070139684E-4</v>
+        <v>2.2719302129656512E-4</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
@@ -1232,11 +1255,11 @@
       </c>
       <c r="B15" s="19">
         <f>D15*1000</f>
-        <v>0.50656872045869017</v>
+        <v>0.23808729861558436</v>
       </c>
       <c r="D15" s="20">
         <f>LN(1/(1-0.9))*D12</f>
-        <v>5.065687204586902E-4</v>
+        <v>2.3808729861558435E-4</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
@@ -1245,11 +1268,11 @@
       </c>
       <c r="B16" s="19">
         <f>D16*1000</f>
-        <v>1.0131374409173801</v>
+        <v>0.47617459723116867</v>
       </c>
       <c r="D16">
         <f>LN(1/(1-0.99))*D12</f>
-        <v>1.0131374409173802E-3</v>
+        <v>4.7617459723116865E-4</v>
       </c>
     </row>
   </sheetData>
@@ -1289,7 +1312,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1305,12 +1328,12 @@
         <v>8</v>
       </c>
       <c r="B1" s="25">
-        <f>'PWM-backlight'!B9</f>
-        <v>62.5</v>
+        <f>'PWM-backlight'!B10</f>
+        <v>250</v>
       </c>
       <c r="D1">
         <f>B1*1000</f>
-        <v>62500</v>
+        <v>250000</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1342,7 +1365,7 @@
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="22">
+      <c r="B4" s="35">
         <v>4.7</v>
       </c>
       <c r="D4">
@@ -1355,11 +1378,11 @@
         <v>12</v>
       </c>
       <c r="B5" s="15">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D5">
         <f>B5/100</f>
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
@@ -1368,37 +1391,37 @@
       </c>
       <c r="B7" s="16">
         <f>D7</f>
-        <v>0.5</v>
+        <v>2.5</v>
       </c>
       <c r="D7">
         <f>D2*D5</f>
-        <v>0.5</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="34" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="17">
         <f>D8*1000</f>
-        <v>8.5105133850304799</v>
+        <v>10.638288113323231</v>
       </c>
       <c r="C8" s="29"/>
       <c r="D8">
         <f>2*D2*(0.5-ABS(D5-0.5))*D13*PI()/2</f>
-        <v>8.5105133850304805E-3</v>
+        <v>1.063828811332323E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="32"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="30">
         <f>D9</f>
-        <v>1.7021026770060961E-2</v>
+        <v>4.2553152453292924E-3</v>
       </c>
       <c r="C9" s="29"/>
       <c r="D9">
         <f>D8/D7</f>
-        <v>1.7021026770060961E-2</v>
+        <v>4.2553152453292924E-3</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
@@ -1407,11 +1430,11 @@
       </c>
       <c r="B10" s="17">
         <f>D10*1000</f>
-        <v>42.552566925152405</v>
+        <v>10.638288113323231</v>
       </c>
       <c r="D10">
         <f>2*D2*0.5*D13*PI()/2</f>
-        <v>4.2552566925152406E-2</v>
+        <v>1.063828811332323E-2</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
@@ -1446,11 +1469,11 @@
       </c>
       <c r="B13" s="18">
         <f>-20*LOG(D13)</f>
-        <v>45.323282358744883</v>
+        <v>57.364362667301208</v>
       </c>
       <c r="D13">
         <f>1/SQRT(1+(D1/D11)^2)</f>
-        <v>5.4179610939093592E-3</v>
+        <v>1.3545089114169163E-3</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">

</xml_diff>